<commit_message>
[2-3] Eigentrust - random / mean init trust vector
</commit_message>
<xml_diff>
--- a/2-3/reputation/local_trust.xlsx
+++ b/2-3/reputation/local_trust.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anima\Documents\Aberdeen\MSc_AI\CS551K_Agents\practicals\code\2-3\reputation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E25AFC4-6A8D-4176-8830-5B59E0609E80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494E4287-0DEE-4D1D-BC6C-16DA52779BB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1548" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,7 +363,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -404,7 +404,7 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[2-3] BRS: decoding and addition
</commit_message>
<xml_diff>
--- a/2-3/reputation/local_trust.xlsx
+++ b/2-3/reputation/local_trust.xlsx
@@ -8,41 +8,55 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anima\Documents\Aberdeen\MSc_AI\CS551K_Agents\practicals\code\2-3\reputation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494E4287-0DEE-4D1D-BC6C-16DA52779BB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BA29D2-42C9-41A9-A3E9-4AF420F5AA6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1548" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1548" windowWidth="6468" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>trustee A0</t>
-  </si>
-  <si>
-    <t>trustee A1</t>
-  </si>
-  <si>
-    <t>trustee A2</t>
-  </si>
-  <si>
-    <t>trustor A0</t>
-  </si>
-  <si>
-    <t>trustor A1</t>
-  </si>
-  <si>
-    <t>trustor A2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>trustee A</t>
+  </si>
+  <si>
+    <t>trustee C</t>
+  </si>
+  <si>
+    <t>trustee D</t>
+  </si>
+  <si>
+    <t>trustor A</t>
+  </si>
+  <si>
+    <t>trustor B</t>
+  </si>
+  <si>
+    <t>trustor C</t>
+  </si>
+  <si>
+    <t>trustor D</t>
+  </si>
+  <si>
+    <t>trustee B</t>
   </si>
 </sst>
 </file>
@@ -360,65 +374,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f>5-(2+1)</f>
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <f>1-0</f>
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>-2</v>
+      <c r="E2">
+        <f>4-3</f>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <f>4-3</f>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <f>7-1</f>
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <f>1-1</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
+        <f>0-0</f>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f>6-2</f>
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>2-3</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <f>0-0</f>
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <f>1-0</f>
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f>4-2</f>
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>-3</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
+      <c r="E5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>